<commit_message>
add head line supported
</commit_message>
<xml_diff>
--- a/src/test/resources/template.xlsx
+++ b/src/test/resources/template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25520" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="25520" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="会员" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -184,6 +184,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -526,7 +529,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.3"/>
@@ -548,9 +551,15 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="2">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
export with specified included fields
</commit_message>
<xml_diff>
--- a/src/test/resources/template.xlsx
+++ b/src/test/resources/template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoohuang/github/excel2javabeans/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoo/GitHub/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63185D0F-8BF8-3044-A165-129FE1469E48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25520" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="5000" yWindow="3960" windowWidth="25520" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="会员" sheetId="1" r:id="rId1"/>
     <sheet name="排期" sheetId="2" r:id="rId2"/>
-    <sheet name="订课" sheetId="3" r:id="rId3"/>
+    <sheet name="订课情况" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -78,8 +79,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,8 +129,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Hiragino Sans GB W3"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +146,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8A6FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,7 +191,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -188,6 +207,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -196,9 +221,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC8A6FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -525,32 +558,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>10</v>
       </c>
@@ -568,14 +601,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -584,7 +617,7 @@
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="17">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -601,714 +634,714 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="23">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="23">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="23">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="23">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="23">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="23">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="23">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="23">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="23">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="23">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="23">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="23">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="23">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="23">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="23">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="23">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="23">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="23">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="23">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="23">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="23">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="23">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="23">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="23">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="23">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="23">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="23">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="23">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="23">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="23">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="23">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="23">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="23">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="23">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="23">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="23">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="23">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="23">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="23">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="23">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="23">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="23">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="23">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="23">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="23">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="23">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="23">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="23">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="23">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="23">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="23">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="23">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
     </row>
-    <row r="54" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="23">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="23">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="23">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="23">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="23">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="23">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="23">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="23">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="23">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="23">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="23">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="23">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="23">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="23">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="23">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="23">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="23">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="23">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="23">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="23">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="23">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="23">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="23">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="23">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="23">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="23">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="23">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="23">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="23">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="23">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="23">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
     </row>
-    <row r="85" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="23">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="23">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="23">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
     </row>
-    <row r="88" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="23">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="23">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="23">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="23">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="23">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="23">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="23">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="23">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
     </row>
-    <row r="96" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="23">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
     </row>
-    <row r="97" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="23">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
     </row>
-    <row r="98" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="23">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
     </row>
-    <row r="99" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="23">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
     </row>
-    <row r="100" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="23">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
     </row>
-    <row r="101" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="23">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
     </row>
-    <row r="102" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="23">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
     </row>
-    <row r="103" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="23">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -1322,19 +1355,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1345,262 +1378,262 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>

</xml_diff>